<commit_message>
added loss graph for different LR
</commit_message>
<xml_diff>
--- a/BackProp.xlsx
+++ b/BackProp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVA8\BackProp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E618024E-6754-4CA8-9711-1D879061A91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A590B6D-BB10-45A6-9BCC-6DBD626C8AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F147710-621A-4421-BDD9-A6A0FF4E0F13}"/>
   </bookViews>
@@ -361,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -375,9 +375,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -387,7 +384,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,7 +930,9 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2054,16 +2055,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>107024</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>231434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>913014</xdr:colOff>
+      <xdr:colOff>933061</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>51954</xdr:rowOff>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2390,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE932F8A-A13F-4D3E-B4EC-75624BAE9B5E}">
   <dimension ref="A1:AQ131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AS1048576"/>
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
@@ -2402,33 +2403,33 @@
   <sheetData>
     <row r="1" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="Y2" s="9" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="Y2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
     </row>
     <row r="3" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
       <c r="Y3" s="6" t="s">
         <v>48</v>
       </c>
@@ -2442,13 +2443,13 @@
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
       <c r="Y4" s="6" t="s">
         <v>49</v>
       </c>
@@ -2462,13 +2463,13 @@
       <c r="AG4" s="6"/>
     </row>
     <row r="5" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
       <c r="Y5" s="6" t="s">
         <v>50</v>
       </c>
@@ -2482,122 +2483,122 @@
       <c r="AG5" s="6"/>
     </row>
     <row r="6" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="Y6" s="8" t="s">
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="Y6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
     </row>
     <row r="7" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="Y7" s="8" t="s">
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="Y7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
     </row>
     <row r="8" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="Y8" s="8" t="s">
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="Y8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
     </row>
     <row r="9" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R9" s="8" t="s">
+      <c r="R9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="Y9" s="8" t="s">
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="Y9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
     </row>
     <row r="10" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="Y10" s="8" t="s">
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="Y10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AN10" s="11"/>
-      <c r="AO10" s="11"/>
-      <c r="AP10" s="11"/>
-      <c r="AQ10" s="11"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
     </row>
     <row r="11" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
       <c r="Y11" s="6" t="s">
         <v>52</v>
       </c>
@@ -2611,13 +2612,13 @@
       <c r="AG11" s="6"/>
     </row>
     <row r="12" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R12" s="8" t="s">
+      <c r="R12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
       <c r="Y12" s="6" t="s">
         <v>65</v>
       </c>
@@ -2629,24 +2630,24 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="11"/>
-      <c r="AO12" s="11"/>
-      <c r="AP12" s="11"/>
-      <c r="AQ12" s="11"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
     </row>
     <row r="13" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="R13" s="8" t="s">
+      <c r="R13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
       <c r="Y13" s="6" t="s">
         <v>66</v>
       </c>
@@ -2658,15 +2659,15 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="6"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="11"/>
-      <c r="AO13" s="11"/>
-      <c r="AP13" s="11"/>
-      <c r="AQ13" s="11"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
     </row>
     <row r="14" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="R14" s="1"/>
@@ -2681,84 +2682,84 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="6"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="11"/>
-      <c r="AO14" s="11"/>
-      <c r="AP14" s="11"/>
-      <c r="AQ14" s="11"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
     </row>
     <row r="15" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="Y15" s="8" t="s">
+      <c r="Y15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
     </row>
     <row r="16" spans="18:43" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="Y16" s="8" t="s">
+      <c r="Y16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
     </row>
     <row r="17" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="Y17" s="8" t="s">
+      <c r="Y17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
     </row>
     <row r="18" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Y18" s="8" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Y18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8"/>
-      <c r="AE18" s="8"/>
-      <c r="AF18" s="8"/>
-      <c r="AG18" s="8"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
     </row>
     <row r="19" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6" t="s">
@@ -2797,17 +2798,17 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
-      <c r="R20" s="9" t="s">
+      <c r="R20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B21" s="6" t="s">
@@ -2887,17 +2888,17 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
-      <c r="R23" s="8" t="s">
+      <c r="R23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B24" s="6" t="s">
@@ -2917,17 +2918,17 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
-      <c r="R24" s="8" t="s">
+      <c r="R24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
     </row>
     <row r="25" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
@@ -2947,17 +2948,17 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
-      <c r="R25" s="8" t="s">
+      <c r="R25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
@@ -15278,33 +15279,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="Y12:AG12"/>
-    <mergeCell ref="Y13:AG13"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="B22:P22"/>
-    <mergeCell ref="Y3:AG3"/>
-    <mergeCell ref="Y4:AG4"/>
-    <mergeCell ref="Y5:AG5"/>
-    <mergeCell ref="Y11:AG11"/>
-    <mergeCell ref="Y16:AG16"/>
-    <mergeCell ref="Y17:AG17"/>
-    <mergeCell ref="Y18:AG18"/>
-    <mergeCell ref="Y14:AG14"/>
-    <mergeCell ref="R20:Z20"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="R11:V11"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="R3:V3"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="R5:V5"/>
-    <mergeCell ref="R6:V6"/>
-    <mergeCell ref="R13:V13"/>
-    <mergeCell ref="R21:Z21"/>
-    <mergeCell ref="R22:Z22"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B24:P24"/>
+    <mergeCell ref="B25:P25"/>
+    <mergeCell ref="B26:P26"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:P19"/>
     <mergeCell ref="R25:Z25"/>
     <mergeCell ref="Y2:AG2"/>
     <mergeCell ref="Y6:AG6"/>
@@ -15316,12 +15296,33 @@
     <mergeCell ref="R24:Z24"/>
     <mergeCell ref="Y15:AG15"/>
     <mergeCell ref="R12:V12"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B26:P26"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="R5:V5"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="R9:V9"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="Y3:AG3"/>
+    <mergeCell ref="Y4:AG4"/>
+    <mergeCell ref="Y5:AG5"/>
+    <mergeCell ref="Y11:AG11"/>
+    <mergeCell ref="Y16:AG16"/>
+    <mergeCell ref="Y14:AG14"/>
+    <mergeCell ref="Y12:AG12"/>
+    <mergeCell ref="Y13:AG13"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:P22"/>
+    <mergeCell ref="Y17:AG17"/>
+    <mergeCell ref="Y18:AG18"/>
+    <mergeCell ref="R20:Z20"/>
+    <mergeCell ref="R13:V13"/>
+    <mergeCell ref="R21:Z21"/>
+    <mergeCell ref="R22:Z22"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="W32:W131">

</xml_diff>